<commit_message>
Removed RawTestData.csv and changed parameters of RawTestData.xlsx
</commit_message>
<xml_diff>
--- a/tests/0TestInput/RawTestData.xlsx
+++ b/tests/0TestInput/RawTestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/tests/0TestInput/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1F1DC1-DC01-7A4A-93EA-87BE437D3ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="26380" windowHeight="13360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Type</t>
   </si>
@@ -61,12 +67,6 @@
     <t>[annual, quarterly, monthly]</t>
   </si>
   <si>
-    <t>500000-1000000,25000</t>
-  </si>
-  <si>
-    <t>10000-50000,5000</t>
-  </si>
-  <si>
     <t>100-1000,200</t>
   </si>
   <si>
@@ -76,26 +76,35 @@
     <t>[20,40,60]</t>
   </si>
   <si>
-    <t>25000-200000,10000</t>
-  </si>
-  <si>
     <t>[1000,300,500]</t>
   </si>
   <si>
     <t>[1,2,3,5]</t>
   </si>
   <si>
-    <t>30000-2500000,20000</t>
-  </si>
-  <si>
     <t>[500,700,1000]</t>
+  </si>
+  <si>
+    <t>[Corporate]</t>
+  </si>
+  <si>
+    <t>500000-1000000,100000</t>
+  </si>
+  <si>
+    <t>10000-50000,10000</t>
+  </si>
+  <si>
+    <t>20000-200000,40000</t>
+  </si>
+  <si>
+    <t>30000-2500000,100000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,15 +137,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -178,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,9 +227,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,6 +279,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,16 +472,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="9" max="9" width="34.6640625" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -471,77 +534,77 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RND_ prefix in raw data update.
</commit_message>
<xml_diff>
--- a/tests/0TestInput/RawTestData.xlsx
+++ b/tests/0TestInput/RawTestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/tests/0TestInput/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1F1DC1-DC01-7A4A-93EA-87BE437D3ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="26380" windowHeight="13360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="24240" windowHeight="13365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,53 +52,53 @@
     <t>[Cov. Type2, Cov. Type3, Cov. Type4]</t>
   </si>
   <si>
-    <t>[2,4,5,7,9]</t>
-  </si>
-  <si>
     <t>[Taxi, Private, Corporate]</t>
   </si>
   <si>
-    <t>[annual, quarterly, monthly]</t>
-  </si>
-  <si>
     <t>100-1000,200</t>
   </si>
   <si>
     <t>[0,1]</t>
   </si>
   <si>
-    <t>[20,40,60]</t>
-  </si>
-  <si>
     <t>[1000,300,500]</t>
   </si>
   <si>
-    <t>[1,2,3,5]</t>
-  </si>
-  <si>
     <t>[500,700,1000]</t>
   </si>
   <si>
     <t>[Corporate]</t>
   </si>
   <si>
-    <t>500000-1000000,100000</t>
-  </si>
-  <si>
-    <t>10000-50000,10000</t>
-  </si>
-  <si>
-    <t>20000-200000,40000</t>
-  </si>
-  <si>
-    <t>30000-2500000,100000</t>
+    <t>RND_[2,4,5,7,9]</t>
+  </si>
+  <si>
+    <t>RND_[20,40,60]</t>
+  </si>
+  <si>
+    <t>RND_[1,2,3,5]</t>
+  </si>
+  <si>
+    <t>RND_500000-1000000,100000</t>
+  </si>
+  <si>
+    <t>RND_[annual, quarterly, monthly]</t>
+  </si>
+  <si>
+    <t>RND_10000-50000,10000</t>
+  </si>
+  <si>
+    <t>RND_20000-200000,40000</t>
+  </si>
+  <si>
+    <t>RND_30000-2500000,100000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,7 +131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -153,7 +147,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -195,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,27 +221,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,24 +255,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -472,26 +430,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="9" max="9" width="34.6640625" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,91 +478,91 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comments added for different data types
</commit_message>
<xml_diff>
--- a/tests/0TestInput/RawTestData.xlsx
+++ b/tests/0TestInput/RawTestData.xlsx
@@ -13,6 +13,870 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Akash</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List of headers:
+In output evert value in this list will be treated as header and the will be assigned below datas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Single value, will be treat as individual and will be added in all other possibilites</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List: In output each value will have every possible combination with other data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from the range list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from the range list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Range: start-end,step
+Create a list of number from start to end with the gap of step</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List: In output each value will have every possible combination with other data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List: In output each value will have every possible combination with other data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FKR_ prefix is used to create fake data.
+Format: FKR(type, locale, num)
+type=type of data
+locale=region_lauguage
+num=num of data in list
+default num=5, 
+if num=0 new data will be generated with each output data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FKR_ prefix is used to create fake data.
+Format: FKR(type, locale, num)
+type=type of data
+locale=region_lauguage
+num=num of data in list
+default num=5, 
+if num=0 new data will be generated with each output data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Single value, will be treat as individual and will be added in all other possibilites</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Single value, will be treat as individual and will be added in all other possibilites</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from the range list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from the range list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List: In output each value will have every possible combination with other data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Single value, will be treat as individual and will be added in all other possibilites</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List: In output each value will have every possible combination with other data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FKR_ prefix is used to create fake data.
+Format: FKR(type, locale, num)
+type=type of data
+locale=region_lauguage
+num=num of data in list
+default num=5, 
+if num=0 new data will be generated with each output data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FKR_ prefix is used to create fake data.
+Format: FKR(type, locale, num)
+type=type of data
+locale=region_lauguage
+num=num of data in list
+default num=5, 
+if num=0 new data will be generated with each output data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Single value, will be treat as individual and will be added in all other possibilites</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Single value, will be treat as individual and will be added in all other possibilites</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from the range list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RND_ prefix picks a random value from the range list instead of creating all possibilites.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List: In output each value will have every possible combination with other data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Single value, will be treat as individual and will be added in all other possibilites</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List: In output each value will have every possible combination with other data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FKR_ prefix is used to create fake data.
+Format: FKR(type, locale, num)
+type=type of data
+locale=region_lauguage
+num=num of data in list
+default num=5, 
+if num=0 new data will be generated with each output data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FKR_ prefix is used to create fake data.
+Format: FKR(type, locale, num)
+type=type of data
+locale=region_lauguage
+num=num of data in list
+default num=5, 
+if num=0 new data will be generated with each output data.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
@@ -119,13 +983,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -454,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -613,5 +1490,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for RRD_ prefix
</commit_message>
<xml_diff>
--- a/tests/0TestInput/RawTestData.xlsx
+++ b/tests/0TestInput/RawTestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="24240" windowHeight="13365"/>
+    <workbookView xWindow="240" yWindow="468" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -321,6 +322,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="L2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a list of TargetData value from matched data. At last it will add random data from the TargarData List in every data of output</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A3" authorId="0">
       <text>
         <r>
@@ -597,6 +623,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="L3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a list of TargetData value from matched data. At last it will add random data from the TargarData List in every data of output</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0">
       <text>
         <r>
@@ -873,12 +924,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a list of TargetData value from matched data. At last it will add random data from the TargarData List in every data of output</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Type</t>
   </si>
@@ -977,6 +1053,48 @@
   </si>
   <si>
     <t>FKR_(email,EN_US ,1)</t>
+  </si>
+  <si>
+    <t>Customer Id</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Employment_status</t>
+  </si>
+  <si>
+    <t>RRD_(Sheet2,Customer,[Age group:[20s],Employment_status:[unemployed]])</t>
+  </si>
+  <si>
+    <t>RRD_(Sheet2,Customer,[Age group:[60s],Employment_status:[employed, unemployed]])</t>
+  </si>
+  <si>
+    <t>RRD_(Sheet2,Customer,[Age group:[30s,40s],Employment_status:[employed]])</t>
+  </si>
+  <si>
+    <t>Age group</t>
+  </si>
+  <si>
+    <t>30s</t>
+  </si>
+  <si>
+    <t>40s</t>
+  </si>
+  <si>
+    <t>60s</t>
+  </si>
+  <si>
+    <t>50s</t>
+  </si>
+  <si>
+    <t>20s</t>
+  </si>
+  <si>
+    <t>unemployed</t>
+  </si>
+  <si>
+    <t>employed</t>
   </si>
 </sst>
 </file>
@@ -1329,26 +1447,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" customWidth="1"/>
+    <col min="9" max="9" width="34.6640625" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" customWidth="1"/>
+    <col min="12" max="12" width="50.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1382,8 +1501,11 @@
       <c r="K1" t="s">
         <v>27</v>
       </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1417,8 +1539,11 @@
       <c r="K2" t="s">
         <v>28</v>
       </c>
+      <c r="L2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1452,8 +1577,11 @@
       <c r="K3" t="s">
         <v>29</v>
       </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1486,6 +1614,9 @@
       </c>
       <c r="K4" t="s">
         <v>30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1493,4 +1624,140 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>30825</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>40999</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>63829</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>58666</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>23958</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>33345</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>23343</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>40555</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>62895</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>33859</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Multifunctinality RRD_ prefix updated
</commit_message>
<xml_diff>
--- a/tests/0TestInput/RawTestData.xlsx
+++ b/tests/0TestInput/RawTestData.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="468" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="3396" yWindow="1836" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Agents" sheetId="4" r:id="rId2"/>
+    <sheet name="PaymentTerms" sheetId="3" r:id="rId3"/>
+    <sheet name="Customers" sheetId="2" r:id="rId4"/>
+    <sheet name="AgentTypeSpecificFields" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -20,31 +23,6 @@
     <author>Akash</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Akash:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-List of headers:
-In output evert value in this list will be treated as header and the will be assigned below datas</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A2" authorId="0">
       <text>
         <r>
@@ -343,7 +321,98 @@
           </rPr>
           <t xml:space="preserve">
 RRD_(sheetName,TargetData,[header:[value],header[value,value]])
-RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a list of TargetData value from matched data. At last it will add random data from the TargarData List in every data of output</t>
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
         </r>
       </text>
     </comment>
@@ -644,7 +713,69 @@
           </rPr>
           <t xml:space="preserve">
 RRD_(sheetName,TargetData,[header:[value],header[value,value]])
-RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a list of TargetData value from matched data. At last it will add random data from the TargarData List in every data of output</t>
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
         </r>
       </text>
     </comment>
@@ -945,7 +1076,69 @@
           </rPr>
           <t xml:space="preserve">
 RRD_(sheetName,TargetData,[header:[value],header[value,value]])
-RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a list of TargetData value from matched data. At last it will add random data from the TargarData List in every data of output</t>
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Akash:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RRD_(sheetName,TargetData,[header:[value],header[value,value]])
+RRD_ prefix will match data specified inside header: value in sheetName. After then it will make a Dictionary of TargetData value from matched data. At last it will add random data from the TargarData Dict in every data of output. 
+If TargetData = * then all data of the matched list will be treated as TargetData Data. 
+If Header: key list is empty(i.e. []) then no data will be matched and TargetData will be taken from whole list.
+If RRD_ prefix is used multiple time and the TargetData name matches of cells then they will be treated as one for both the output.
+And random selection of both will have same data whos header are matching.</t>
         </r>
       </text>
     </comment>
@@ -954,7 +1147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
   <si>
     <t>Type</t>
   </si>
@@ -1055,24 +1248,12 @@
     <t>FKR_(email,EN_US ,1)</t>
   </si>
   <si>
-    <t>Customer Id</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
     <t>Employment_status</t>
   </si>
   <si>
-    <t>RRD_(Sheet2,Customer,[Age group:[20s],Employment_status:[unemployed]])</t>
-  </si>
-  <si>
-    <t>RRD_(Sheet2,Customer,[Age group:[60s],Employment_status:[employed, unemployed]])</t>
-  </si>
-  <si>
-    <t>RRD_(Sheet2,Customer,[Age group:[30s,40s],Employment_status:[employed]])</t>
-  </si>
-  <si>
     <t>Age group</t>
   </si>
   <si>
@@ -1095,13 +1276,115 @@
   </si>
   <si>
     <t>employed</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>BankID</t>
+  </si>
+  <si>
+    <t>BankAccount</t>
+  </si>
+  <si>
+    <t>CardCompany</t>
+  </si>
+  <si>
+    <t>CardValidTo</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Amex</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>05/20</t>
+  </si>
+  <si>
+    <t>06/21</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>03/24</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>RRD_[PaymentTerms, *,[]]</t>
+  </si>
+  <si>
+    <t>RRD_(Customers,Customer,[Age group:[60s],Employment_status:[employed, unemployed]])</t>
+  </si>
+  <si>
+    <t>RRD_(Customers,Customer,[Age group:[20s],Employment_status:[unemployed]])</t>
+  </si>
+  <si>
+    <t>RRD_(Customers,Customer,[Age group:[30s,40s],Employment_status:[employed]])</t>
+  </si>
+  <si>
+    <t>Agents</t>
+  </si>
+  <si>
+    <t>Agenttype</t>
+  </si>
+  <si>
+    <t>Agent#</t>
+  </si>
+  <si>
+    <t>Own</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>9 Years</t>
+  </si>
+  <si>
+    <t>10 Years</t>
+  </si>
+  <si>
+    <t>1 Year</t>
+  </si>
+  <si>
+    <t>11 Years</t>
+  </si>
+  <si>
+    <t>AdditionalFieldsAgent</t>
+  </si>
+  <si>
+    <t>RRD_[Agents, *, [Agenttype:[Own, Partner]]]</t>
+  </si>
+  <si>
+    <t>RRD_[AgentTypeSpecificFields,*,[Agenttype:[Own, Partner]]]</t>
+  </si>
+  <si>
+    <t>RRD_[PaymentTerms, *,[PaymentType:[Card]]]</t>
+  </si>
+  <si>
+    <t>RRD_[PaymentTerms, *,[PaymentType:[Bank]]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1110,13 +1393,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1143,8 +1433,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1447,15 +1740,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" activeCellId="3" sqref="L3 L4 M2 N2:O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
     <col min="4" max="4" width="29.44140625" customWidth="1"/>
     <col min="5" max="5" width="23.109375" customWidth="1"/>
@@ -1463,11 +1756,14 @@
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="9" max="9" width="34.6640625" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" customWidth="1"/>
-    <col min="12" max="12" width="50.88671875" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="44.33203125" customWidth="1"/>
+    <col min="13" max="13" width="61.109375" customWidth="1"/>
+    <col min="14" max="14" width="69" customWidth="1"/>
+    <col min="15" max="15" width="38.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1502,10 +1798,19 @@
         <v>27</v>
       </c>
       <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1540,10 +1845,19 @@
         <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>73</v>
+      </c>
+      <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1578,10 +1892,16 @@
         <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>73</v>
+      </c>
+      <c r="N3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1616,7 +1936,13 @@
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>73</v>
+      </c>
+      <c r="N4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1628,23 +1954,198 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>1234123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>12312312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>6542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>8752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>1234123131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>45341</v>
+      </c>
+      <c r="C3">
+        <v>9824412389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>45119</v>
+      </c>
+      <c r="C4">
+        <v>9923130010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>1234131</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6">
+        <v>123999</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <v>123123</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1652,10 +2153,10 @@
         <v>30825</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1663,10 +2164,10 @@
         <v>40999</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1674,10 +2175,10 @@
         <v>63829</v>
       </c>
       <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1685,10 +2186,10 @@
         <v>58666</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1696,10 +2197,10 @@
         <v>23958</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1707,10 +2208,10 @@
         <v>33345</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1718,10 +2219,10 @@
         <v>23343</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1729,10 +2230,10 @@
         <v>40555</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1740,10 +2241,10 @@
         <v>62895</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1751,13 +2252,68 @@
         <v>33859</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Prcessing values after final testcase dict is created, updated TDG unit test & test input file
</commit_message>
<xml_diff>
--- a/tests/0TestInput/RawTestData.xlsx
+++ b/tests/0TestInput/RawTestData.xlsx
@@ -1415,10 +1415,10 @@
     <t>Test Renv</t>
   </si>
   <si>
-    <t>RRE_[../../examples/CompleteBaangtWebdemo.xlsx,CustomerData,[NameFirst,NameLast],[Stage:[Test]]]</t>
-  </si>
-  <si>
-    <t>Renv_( Usernme)</t>
+    <t>RRE_[examples/CompleteBaangtWebdemo.xlsx,CustomerData,[NameFirst,NameLast],[Stage:[Test]]]</t>
+  </si>
+  <si>
+    <t>Renv_(USERNAME, Test)</t>
   </si>
 </sst>
 </file>

</xml_diff>